<commit_message>
Define RSD space heating commodity groups
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D6EC06-CAFD-4669-8E22-3A4E307F0B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E8AD8F-A1E8-4DF2-BE9B-CBF794FF85CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="28" r:id="rId1"/>
     <sheet name="Regions" sheetId="27" r:id="rId2"/>
     <sheet name="Region Definition" sheetId="20" r:id="rId3"/>
     <sheet name="TimePeriods" sheetId="24" r:id="rId4"/>
-    <sheet name="Import Settings" sheetId="17" r:id="rId5"/>
-    <sheet name="Interpol_Extrapol_Defaults" sheetId="14" r:id="rId6"/>
-    <sheet name="Constants" sheetId="25" r:id="rId7"/>
-    <sheet name="Defaults" sheetId="26" r:id="rId8"/>
-    <sheet name="CPI" sheetId="23" r:id="rId9"/>
+    <sheet name="CGs" sheetId="29" r:id="rId5"/>
+    <sheet name="Import Settings" sheetId="17" r:id="rId6"/>
+    <sheet name="Interpol_Extrapol_Defaults" sheetId="14" r:id="rId7"/>
+    <sheet name="Constants" sheetId="25" r:id="rId8"/>
+    <sheet name="Defaults" sheetId="26" r:id="rId9"/>
+    <sheet name="CPI" sheetId="23" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
@@ -114,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="171">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -618,6 +619,33 @@
   </si>
   <si>
     <t>MEUR2018</t>
+  </si>
+  <si>
+    <t>~TFM_COMGRP</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>RSDSH_APT</t>
+  </si>
+  <si>
+    <t>Residential space heating - apartments</t>
+  </si>
+  <si>
+    <t>RSDSH_ATT</t>
+  </si>
+  <si>
+    <t>RSDSH_DET</t>
+  </si>
+  <si>
+    <t>Residential space heating - detached houses</t>
+  </si>
+  <si>
+    <t>Residential space heating - attached houses</t>
   </si>
 </sst>
 </file>
@@ -3696,9 +3724,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3736,9 +3764,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3771,26 +3799,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3823,26 +3834,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6865,6 +6859,302 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="B2:D26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="4" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="28"/>
+      <c r="C2" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B3" s="31">
+        <v>2000</v>
+      </c>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B4" s="31">
+        <v>2001</v>
+      </c>
+      <c r="C4" s="33">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D4" s="32">
+        <f t="shared" ref="D4:D22" si="0">D3+D3*C4</f>
+        <v>102.2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B5" s="31">
+        <v>2002</v>
+      </c>
+      <c r="C5" s="33">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="D5" s="34">
+        <f t="shared" si="0"/>
+        <v>104.34620000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B6" s="31">
+        <v>2003</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="D6" s="34">
+        <f t="shared" si="0"/>
+        <v>106.43312400000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B7" s="31">
+        <v>2004</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0.02</v>
+      </c>
+      <c r="D7" s="34">
+        <f t="shared" si="0"/>
+        <v>108.56178648000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B8" s="31">
+        <v>2005</v>
+      </c>
+      <c r="C8" s="33">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D8" s="34">
+        <f t="shared" si="0"/>
+        <v>110.95014578256001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B9" s="31">
+        <v>2006</v>
+      </c>
+      <c r="C9" s="33">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D9" s="34">
+        <f t="shared" si="0"/>
+        <v>113.39104898977634</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B10" s="31">
+        <v>2007</v>
+      </c>
+      <c r="C10" s="33">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D10" s="34">
+        <f t="shared" si="0"/>
+        <v>115.99904311654119</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B11" s="31">
+        <v>2008</v>
+      </c>
+      <c r="C11" s="33">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D11" s="34">
+        <f t="shared" si="0"/>
+        <v>120.29100771185321</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B12" s="31">
+        <v>2009</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0.01</v>
+      </c>
+      <c r="D12" s="34">
+        <f t="shared" si="0"/>
+        <v>121.49391778897174</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B13" s="31">
+        <v>2010</v>
+      </c>
+      <c r="C13" s="33">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="D13" s="34">
+        <f t="shared" si="0"/>
+        <v>124.04529006254015</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B14" s="31">
+        <v>2011</v>
+      </c>
+      <c r="C14" s="33">
+        <v>3.1E-2</v>
+      </c>
+      <c r="D14" s="34">
+        <f t="shared" si="0"/>
+        <v>127.89069405447889</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B15" s="31">
+        <v>2012</v>
+      </c>
+      <c r="C15" s="33">
+        <v>2.6000000000000002E-2</v>
+      </c>
+      <c r="D15" s="34">
+        <f t="shared" si="0"/>
+        <v>131.21585209989533</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B16" s="31">
+        <v>2013</v>
+      </c>
+      <c r="C16" s="33">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D16" s="34">
+        <f t="shared" si="0"/>
+        <v>133.18408988139376</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B17" s="31">
+        <v>2014</v>
+      </c>
+      <c r="C17" s="33">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D17" s="34">
+        <f t="shared" si="0"/>
+        <v>133.98319442068211</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B18" s="31">
+        <v>2015</v>
+      </c>
+      <c r="C18" s="38">
+        <v>1E-3</v>
+      </c>
+      <c r="D18" s="34">
+        <f>D17+D17*C18</f>
+        <v>134.1171776151028</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B19" s="36">
+        <v>2016</v>
+      </c>
+      <c r="C19" s="33">
+        <v>2E-3</v>
+      </c>
+      <c r="D19" s="37">
+        <f t="shared" si="0"/>
+        <v>134.385411970333</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B20" s="36">
+        <v>2017</v>
+      </c>
+      <c r="C20" s="33">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="D20" s="37">
+        <f t="shared" si="0"/>
+        <v>136.66996397382866</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B21" s="36">
+        <v>2018</v>
+      </c>
+      <c r="C21" s="33">
+        <v>1.9E-2</v>
+      </c>
+      <c r="D21" s="37">
+        <f t="shared" si="0"/>
+        <v>139.26669328933141</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B22" s="36">
+        <v>2019</v>
+      </c>
+      <c r="C22" s="33">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D22" s="37">
+        <f t="shared" si="0"/>
+        <v>141.35569368867138</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B23" s="36">
+        <v>2020</v>
+      </c>
+      <c r="C23" s="33">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="D23" s="37">
+        <f t="shared" ref="D23" si="1">D22+D22*C23</f>
+        <v>142.34518354449207</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B24" s="36">
+        <v>2021</v>
+      </c>
+      <c r="C24" s="38">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="D24" s="37">
+        <f t="shared" ref="D24" si="2">D23+D23*C24</f>
+        <v>146.47319386728233</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B26" s="35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
@@ -7824,7 +8114,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B3:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
@@ -8420,6 +8710,111 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A232327-7551-4D4C-AA69-4D8DB0F0DCB7}">
+  <dimension ref="B3:Q7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B3" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+    </row>
+    <row r="4" spans="2:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" t="str">
+        <f>_xlfn.TEXTJOIN("",TRUE,B5,"-*")</f>
+        <v>RSDSH_APT-*</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" ref="D6:D7" si="0">_xlfn.TEXTJOIN("",TRUE,B6,"-*")</f>
+        <v>RSDSH_ATT-*</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>RSDSH_DET-*</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B3:C9"/>
@@ -8493,13 +8888,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="A14" sqref="A14:P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8901,7 +9296,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="B1:G34"/>
@@ -9365,7 +9760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="B2:O25"/>
@@ -9717,300 +10112,4 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr codeName="Sheet8"/>
-  <dimension ref="B2:D26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="4" width="13.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="28"/>
-      <c r="C2" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B3" s="31">
-        <v>2000</v>
-      </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B4" s="31">
-        <v>2001</v>
-      </c>
-      <c r="C4" s="33">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="D4" s="32">
-        <f t="shared" ref="D4:D22" si="0">D3+D3*C4</f>
-        <v>102.2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="31">
-        <v>2002</v>
-      </c>
-      <c r="C5" s="33">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="D5" s="34">
-        <f t="shared" si="0"/>
-        <v>104.34620000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B6" s="31">
-        <v>2003</v>
-      </c>
-      <c r="C6" s="33">
-        <v>0.02</v>
-      </c>
-      <c r="D6" s="34">
-        <f t="shared" si="0"/>
-        <v>106.43312400000001</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="31">
-        <v>2004</v>
-      </c>
-      <c r="C7" s="33">
-        <v>0.02</v>
-      </c>
-      <c r="D7" s="34">
-        <f t="shared" si="0"/>
-        <v>108.56178648000001</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B8" s="31">
-        <v>2005</v>
-      </c>
-      <c r="C8" s="33">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="D8" s="34">
-        <f t="shared" si="0"/>
-        <v>110.95014578256001</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" s="31">
-        <v>2006</v>
-      </c>
-      <c r="C9" s="33">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="D9" s="34">
-        <f t="shared" si="0"/>
-        <v>113.39104898977634</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B10" s="31">
-        <v>2007</v>
-      </c>
-      <c r="C10" s="33">
-        <v>2.3E-2</v>
-      </c>
-      <c r="D10" s="34">
-        <f t="shared" si="0"/>
-        <v>115.99904311654119</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B11" s="31">
-        <v>2008</v>
-      </c>
-      <c r="C11" s="33">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="D11" s="34">
-        <f t="shared" si="0"/>
-        <v>120.29100771185321</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B12" s="31">
-        <v>2009</v>
-      </c>
-      <c r="C12" s="33">
-        <v>0.01</v>
-      </c>
-      <c r="D12" s="34">
-        <f t="shared" si="0"/>
-        <v>121.49391778897174</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="31">
-        <v>2010</v>
-      </c>
-      <c r="C13" s="33">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="D13" s="34">
-        <f t="shared" si="0"/>
-        <v>124.04529006254015</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14" s="31">
-        <v>2011</v>
-      </c>
-      <c r="C14" s="33">
-        <v>3.1E-2</v>
-      </c>
-      <c r="D14" s="34">
-        <f t="shared" si="0"/>
-        <v>127.89069405447889</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B15" s="31">
-        <v>2012</v>
-      </c>
-      <c r="C15" s="33">
-        <v>2.6000000000000002E-2</v>
-      </c>
-      <c r="D15" s="34">
-        <f t="shared" si="0"/>
-        <v>131.21585209989533</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B16" s="31">
-        <v>2013</v>
-      </c>
-      <c r="C16" s="33">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="D16" s="34">
-        <f t="shared" si="0"/>
-        <v>133.18408988139376</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B17" s="31">
-        <v>2014</v>
-      </c>
-      <c r="C17" s="33">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="D17" s="34">
-        <f t="shared" si="0"/>
-        <v>133.98319442068211</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B18" s="31">
-        <v>2015</v>
-      </c>
-      <c r="C18" s="38">
-        <v>1E-3</v>
-      </c>
-      <c r="D18" s="34">
-        <f>D17+D17*C18</f>
-        <v>134.1171776151028</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B19" s="36">
-        <v>2016</v>
-      </c>
-      <c r="C19" s="33">
-        <v>2E-3</v>
-      </c>
-      <c r="D19" s="37">
-        <f t="shared" si="0"/>
-        <v>134.385411970333</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B20" s="36">
-        <v>2017</v>
-      </c>
-      <c r="C20" s="33">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="D20" s="37">
-        <f t="shared" si="0"/>
-        <v>136.66996397382866</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B21" s="36">
-        <v>2018</v>
-      </c>
-      <c r="C21" s="33">
-        <v>1.9E-2</v>
-      </c>
-      <c r="D21" s="37">
-        <f t="shared" si="0"/>
-        <v>139.26669328933141</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B22" s="36">
-        <v>2019</v>
-      </c>
-      <c r="C22" s="33">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="D22" s="37">
-        <f t="shared" si="0"/>
-        <v>141.35569368867138</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B23" s="36">
-        <v>2020</v>
-      </c>
-      <c r="C23" s="33">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="D23" s="37">
-        <f t="shared" ref="D23" si="1">D22+D22*C23</f>
-        <v>142.34518354449207</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B24" s="36">
-        <v>2021</v>
-      </c>
-      <c r="C24" s="38">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="D24" s="37">
-        <f t="shared" ref="D24" si="2">D23+D23*C24</f>
-        <v>146.47319386728233</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B26" s="35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-</worksheet>
 </file>
</xml_diff>